<commit_message>
Documentation update and SQL create tables
</commit_message>
<xml_diff>
--- a/Documentation/Data Dictionary.xlsx
+++ b/Documentation/Data Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="53">
   <si>
     <t>Field Name</t>
   </si>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,9 +704,6 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
       <c r="J3" t="s">
         <v>38</v>
       </c>
@@ -724,6 +721,9 @@
       </c>
       <c r="C4">
         <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
@@ -1043,12 +1043,6 @@
       <c r="B25" t="s">
         <v>37</v>
       </c>
-      <c r="J25" t="s">
-        <v>38</v>
-      </c>
-      <c r="K25" t="s">
-        <v>38</v>
-      </c>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1057,9 +1051,6 @@
       </c>
       <c r="B26" t="s">
         <v>37</v>
-      </c>
-      <c r="L26" t="s">
-        <v>38</v>
       </c>
       <c r="N26" s="4"/>
     </row>

</xml_diff>

<commit_message>
View Last 10 Results
User can now view their last 10 test results. Also saving the TestID to
record keeping purposes
</commit_message>
<xml_diff>
--- a/Documentation/Data Dictionary.xlsx
+++ b/Documentation/Data Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="53">
   <si>
     <t>Field Name</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>18,2</t>
+  </si>
+  <si>
+    <t>For record keeping</t>
   </si>
 </sst>
 </file>
@@ -599,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,128 +923,130 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
       </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="6"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" t="s">
-        <v>37</v>
-      </c>
-      <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
@@ -1053,590 +1058,602 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" t="s">
+        <v>37</v>
+      </c>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="N26" s="4"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="6"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31" t="s">
-        <v>37</v>
-      </c>
-      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" t="s">
+        <v>37</v>
+      </c>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>38</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>100</v>
       </c>
-      <c r="N32" s="4"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="6"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="J37" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" t="s">
-        <v>37</v>
-      </c>
-      <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38">
-        <v>1000</v>
+        <v>36</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
       </c>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
       <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40">
         <v>500</v>
       </c>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="6"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
-        <v>36</v>
-      </c>
-      <c r="J44" t="s">
-        <v>37</v>
-      </c>
-      <c r="K44" t="s">
-        <v>37</v>
-      </c>
-      <c r="N44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
       </c>
-      <c r="L45" t="s">
+      <c r="J45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" t="s">
         <v>37</v>
       </c>
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L46" t="s">
+        <v>37</v>
+      </c>
+      <c r="N46" s="4"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N46" s="4" t="s">
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="N47" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="6"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="6"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-      <c r="J51" t="s">
-        <v>37</v>
-      </c>
-      <c r="K51" t="s">
-        <v>37</v>
-      </c>
-      <c r="N51" s="4"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52">
-        <v>100</v>
+        <v>36</v>
+      </c>
+      <c r="J52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
       </c>
       <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
         <v>38</v>
       </c>
       <c r="C53">
+        <v>100</v>
+      </c>
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54">
         <v>500</v>
       </c>
-      <c r="N53" s="4"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-    </row>
-    <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="N54" s="4"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="6"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L57" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="M58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N57" s="1" t="s">
+      <c r="N58" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>36</v>
-      </c>
-      <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
       </c>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>34</v>
+      </c>
+      <c r="N60" s="4"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>32</v>
       </c>
-      <c r="N60" s="4"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
+      <c r="N61" s="4"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AccountManagementForm complete. Title is now Rank.
</commit_message>
<xml_diff>
--- a/Documentation/Data Dictionary.xlsx
+++ b/Documentation/Data Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
   <si>
     <t>Field Name</t>
   </si>
@@ -88,12 +88,6 @@
     <t>AccomplishDate</t>
   </si>
   <si>
-    <t>UserTitles</t>
-  </si>
-  <si>
-    <t>TitleID</t>
-  </si>
-  <si>
     <t>TestData</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>RequiredWPM</t>
   </si>
   <si>
-    <t>TitleName</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -151,9 +142,6 @@
     <t>WPM</t>
   </si>
   <si>
-    <t>Need to create formula. Was thinking it should take about 500 te</t>
-  </si>
-  <si>
     <t>DataSource</t>
   </si>
   <si>
@@ -173,6 +161,15 @@
   </si>
   <si>
     <t>For record keeping</t>
+  </si>
+  <si>
+    <t>RankInfo</t>
+  </si>
+  <si>
+    <t>RankID</t>
+  </si>
+  <si>
+    <t>RankName</t>
   </si>
 </sst>
 </file>
@@ -602,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,10 +690,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -705,10 +702,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -717,16 +714,16 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -735,7 +732,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -747,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -756,40 +753,40 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -798,10 +795,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>150</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -890,10 +890,10 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -902,10 +902,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -914,54 +914,54 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N20" s="4"/>
     </row>
@@ -1049,10 +1049,10 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N25" s="4"/>
     </row>
@@ -1061,10 +1061,10 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -1073,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N27" s="4"/>
     </row>
@@ -1161,143 +1161,140 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
       <c r="C33">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>500</v>
+      </c>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="6"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="J38" t="s">
-        <v>37</v>
-      </c>
-      <c r="K38" t="s">
-        <v>37</v>
-      </c>
-      <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39">
-        <v>1000</v>
+        <v>33</v>
+      </c>
+      <c r="J39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" t="s">
+        <v>34</v>
       </c>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40">
-        <v>500</v>
+        <v>33</v>
       </c>
       <c r="N40" s="4"/>
     </row>
@@ -1320,7 +1317,7 @@
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1382,278 +1379,270 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
       </c>
       <c r="L46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" t="s">
-        <v>36</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="6"/>
+    </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="6"/>
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" t="s">
+        <v>34</v>
+      </c>
+      <c r="K51" t="s">
+        <v>34</v>
+      </c>
+      <c r="N51" s="4"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
-      </c>
-      <c r="J52" t="s">
-        <v>37</v>
-      </c>
-      <c r="K52" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
       </c>
       <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C53">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="N53" s="4"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>40</v>
-      </c>
-      <c r="B54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C54">
-        <v>500</v>
-      </c>
-      <c r="N54" s="4"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-    </row>
-    <row r="56" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="6"/>
+    </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="6"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N60" s="4"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>32</v>
-      </c>
-      <c r="N61" s="4"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F66" s="3"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XP Calculation and Display
User can now calculate and view how much XP they will receive.
Still need to actually add methods to level up.
</commit_message>
<xml_diff>
--- a/Documentation/Data Dictionary.xlsx
+++ b/Documentation/Data Dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="56">
   <si>
     <t>Field Name</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>RankName</t>
+  </si>
+  <si>
+    <t>XPModifierInfo</t>
+  </si>
+  <si>
+    <t>ModifierType</t>
+  </si>
+  <si>
+    <t>RequiredValue</t>
+  </si>
+  <si>
+    <t>ModifierValue</t>
   </si>
 </sst>
 </file>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1329,7 @@
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1379,149 +1391,146 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
-      </c>
-      <c r="J45" t="s">
-        <v>34</v>
-      </c>
-      <c r="K45" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
       </c>
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46">
-        <v>50</v>
-      </c>
-      <c r="L46" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
       </c>
       <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="6"/>
-    </row>
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="N47" s="4"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="6"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N50" s="1" t="s">
+      <c r="N51" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" t="s">
-        <v>33</v>
-      </c>
-      <c r="J51" t="s">
-        <v>34</v>
-      </c>
-      <c r="K51" t="s">
-        <v>34</v>
-      </c>
-      <c r="N51" s="4"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52">
-        <v>100</v>
+        <v>33</v>
+      </c>
+      <c r="J52" t="s">
+        <v>34</v>
+      </c>
+      <c r="K52" t="s">
+        <v>34</v>
       </c>
       <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>35</v>
       </c>
       <c r="C53">
-        <v>500</v>
+        <v>50</v>
+      </c>
+      <c r="L53" t="s">
+        <v>34</v>
       </c>
       <c r="N53" s="4"/>
     </row>
@@ -1544,7 +1553,7 @@
     <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1611,17 +1620,35 @@
       <c r="B58" t="s">
         <v>33</v>
       </c>
+      <c r="J58" t="s">
+        <v>34</v>
+      </c>
+      <c r="K58" t="s">
+        <v>34</v>
+      </c>
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
       </c>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60">
+        <v>500</v>
       </c>
       <c r="N60" s="4"/>
     </row>
@@ -1641,8 +1668,108 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F65" s="3"/>
+    <row r="62" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="N65" s="4"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" s="4"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="N67" s="4"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F72" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>